<commit_message>
Lots of bugs and bug fixes
Working on implementation of keyboard input. Having difficulty closing listener for input. Some major improvements to audio, hints, repeating questions, graphics, and updates to the main spreadsheet.
</commit_message>
<xml_diff>
--- a/answer_sheets/L4AS.xlsx
+++ b/answer_sheets/L4AS.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Caelan\Documents\Japanese_SpeechProgram\answer_sheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Caelan\Documents\GitHub\JapaneseSpeechProgram\answer_sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F4B7DD7-3C17-4D01-823D-86322BB6C419}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0664D9C-ECAE-4932-A85E-7554280B2608}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A85B96A8-BC77-4CE1-99B3-3D42F1408ABE}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="100">
   <si>
     <t>はい元気です</t>
   </si>
@@ -104,9 +104,6 @@
     <t>歳です</t>
   </si>
   <si>
-    <t>TIME_REUSABLE</t>
-  </si>
-  <si>
     <t>GENERAL_QUESTION</t>
   </si>
   <si>
@@ -116,9 +113,6 @@
     <t>LESSON_2</t>
   </si>
   <si>
-    <t>OBJECT_REUSABLE</t>
-  </si>
-  <si>
     <t>Sorewanandesuka?</t>
   </si>
   <si>
@@ -291,6 +285,54 @@
   </si>
   <si>
     <t>GREETINGS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Update </t>
+  </si>
+  <si>
+    <t>コンピューター</t>
+  </si>
+  <si>
+    <t>今は12時半です</t>
+  </si>
+  <si>
+    <t>じゅうにじ。。。</t>
+  </si>
+  <si>
+    <t>How old are you?</t>
+  </si>
+  <si>
+    <t>How are you?</t>
+  </si>
+  <si>
+    <t>Where is the café?</t>
+  </si>
+  <si>
+    <t>Where is the hospital?</t>
+  </si>
+  <si>
+    <t>Where is the bank?</t>
+  </si>
+  <si>
+    <t>Where is the supermarket?</t>
+  </si>
+  <si>
+    <t>Where is the department store.</t>
+  </si>
+  <si>
+    <t>Where is the park?</t>
+  </si>
+  <si>
+    <t>Where is the post office?</t>
+  </si>
+  <si>
+    <t>病院は喫茶店の右だし</t>
+  </si>
+  <si>
+    <t>attention.png</t>
+  </si>
+  <si>
+    <t>げんきですか？</t>
   </si>
 </sst>
 </file>
@@ -674,10 +716,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4ADC8BB-A32A-472F-9CBF-88915A0B884F}">
-  <dimension ref="A1:U11"/>
+  <dimension ref="A1:V11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D4"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -688,7 +730,7 @@
     <col min="4" max="21" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -696,94 +738,103 @@
         <v>20</v>
       </c>
       <c r="C1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D1" t="s">
-        <v>85</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>0</v>
+        <v>83</v>
+      </c>
+      <c r="E1" t="s">
+        <v>98</v>
+      </c>
+      <c r="F1" t="s">
+        <v>89</v>
+      </c>
+      <c r="G1" t="s">
+        <v>99</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="Q1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>13</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B2" t="s">
         <v>20</v>
       </c>
       <c r="C2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D2" t="s">
-        <v>26</v>
+        <v>84</v>
       </c>
       <c r="E2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F2" t="s">
-        <v>27</v>
-      </c>
-      <c r="G2" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="M2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="M2" s="1"/>
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
       <c r="P2" s="1"/>
+      <c r="Q2" s="1"/>
     </row>
-    <row r="3" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>19</v>
       </c>
@@ -791,25 +842,28 @@
         <v>20</v>
       </c>
       <c r="C3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F3" t="s">
-        <v>23</v>
-      </c>
-      <c r="G3" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>17</v>
       </c>
+      <c r="J3" t="s">
+        <v>86</v>
+      </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -817,286 +871,316 @@
         <v>21</v>
       </c>
       <c r="C4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D4" t="s">
-        <v>26</v>
-      </c>
-      <c r="G4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" t="s">
+        <v>98</v>
+      </c>
+      <c r="F4" t="s">
+        <v>88</v>
+      </c>
+      <c r="H4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B5" t="s">
         <v>20</v>
       </c>
       <c r="C5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E5" t="s">
         <v>32</v>
       </c>
-      <c r="D5" t="s">
+      <c r="F5" t="s">
+        <v>90</v>
+      </c>
+      <c r="H5" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E5" t="s">
+      <c r="I5" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="J5" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="K5" t="s">
         <v>36</v>
       </c>
-      <c r="I5" s="1" t="s">
+      <c r="L5" t="s">
         <v>37</v>
       </c>
-      <c r="J5" t="s">
+      <c r="M5" t="s">
         <v>38</v>
       </c>
-      <c r="K5" t="s">
+      <c r="N5" t="s">
         <v>39</v>
       </c>
-      <c r="L5" t="s">
+      <c r="O5" t="s">
+        <v>33</v>
+      </c>
+      <c r="P5" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>46</v>
+      </c>
+      <c r="R5" t="s">
+        <v>46</v>
+      </c>
+      <c r="S5" t="s">
+        <v>47</v>
+      </c>
+      <c r="T5" t="s">
+        <v>48</v>
+      </c>
+      <c r="U5" t="s">
+        <v>81</v>
+      </c>
+      <c r="V5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>40</v>
-      </c>
-      <c r="M5" t="s">
-        <v>41</v>
-      </c>
-      <c r="N5" t="s">
-        <v>35</v>
-      </c>
-      <c r="O5" t="s">
-        <v>39</v>
-      </c>
-      <c r="P5" t="s">
-        <v>48</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>48</v>
-      </c>
-      <c r="R5" t="s">
-        <v>49</v>
-      </c>
-      <c r="S5" t="s">
-        <v>50</v>
-      </c>
-      <c r="T5" t="s">
-        <v>83</v>
-      </c>
-      <c r="U5" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="6" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>42</v>
       </c>
       <c r="B6" t="s">
         <v>20</v>
       </c>
       <c r="C6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E6" t="s">
         <v>32</v>
       </c>
-      <c r="D6" t="s">
-        <v>33</v>
-      </c>
-      <c r="E6" t="s">
-        <v>34</v>
-      </c>
-      <c r="G6" t="s">
+      <c r="F6" t="s">
+        <v>91</v>
+      </c>
+      <c r="H6" t="s">
+        <v>41</v>
+      </c>
+      <c r="I6" t="s">
+        <v>42</v>
+      </c>
+      <c r="J6" t="s">
         <v>43</v>
       </c>
-      <c r="H6" t="s">
+      <c r="K6" t="s">
+        <v>45</v>
+      </c>
+      <c r="L6" t="s">
         <v>44</v>
       </c>
-      <c r="I6" t="s">
-        <v>45</v>
-      </c>
-      <c r="J6" t="s">
-        <v>47</v>
-      </c>
-      <c r="K6" t="s">
-        <v>46</v>
-      </c>
-      <c r="L6" t="s">
-        <v>43</v>
+      <c r="M6" t="s">
+        <v>41</v>
+      </c>
+      <c r="N6" t="s">
+        <v>97</v>
       </c>
     </row>
-    <row r="7" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B7" t="s">
         <v>20</v>
       </c>
       <c r="C7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E7" t="s">
         <v>32</v>
       </c>
-      <c r="D7" t="s">
-        <v>33</v>
-      </c>
-      <c r="E7" t="s">
-        <v>34</v>
-      </c>
-      <c r="G7" s="1" t="s">
+      <c r="F7" t="s">
+        <v>92</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="J7" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="K7" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="I7" s="1" t="s">
+      <c r="L7" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="J7" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="K7" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="L7" s="1"/>
       <c r="M7" s="1"/>
       <c r="N7" s="1"/>
       <c r="O7" s="1"/>
+      <c r="P7" s="1"/>
     </row>
-    <row r="8" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B8" t="s">
         <v>20</v>
       </c>
       <c r="C8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" t="s">
+        <v>31</v>
+      </c>
+      <c r="E8" t="s">
         <v>32</v>
       </c>
-      <c r="D8" t="s">
-        <v>33</v>
-      </c>
-      <c r="E8" t="s">
-        <v>34</v>
-      </c>
-      <c r="G8" t="s">
+      <c r="F8" t="s">
+        <v>94</v>
+      </c>
+      <c r="H8" t="s">
+        <v>56</v>
+      </c>
+      <c r="I8" t="s">
+        <v>57</v>
+      </c>
+      <c r="J8" t="s">
         <v>58</v>
       </c>
-      <c r="H8" t="s">
+      <c r="K8" t="s">
         <v>59</v>
       </c>
-      <c r="I8" t="s">
+      <c r="L8" t="s">
         <v>60</v>
       </c>
-      <c r="J8" t="s">
+      <c r="M8" t="s">
         <v>61</v>
       </c>
-      <c r="K8" t="s">
+      <c r="N8" t="s">
+        <v>63</v>
+      </c>
+      <c r="O8" t="s">
+        <v>57</v>
+      </c>
+      <c r="P8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>62</v>
-      </c>
-      <c r="L8" t="s">
-        <v>63</v>
-      </c>
-      <c r="M8" t="s">
-        <v>65</v>
-      </c>
-      <c r="N8" t="s">
-        <v>59</v>
-      </c>
-      <c r="O8" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="9" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>64</v>
       </c>
       <c r="B9" t="s">
         <v>20</v>
       </c>
       <c r="C9" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" t="s">
+        <v>31</v>
+      </c>
+      <c r="E9" t="s">
         <v>32</v>
       </c>
-      <c r="D9" t="s">
-        <v>33</v>
-      </c>
-      <c r="E9" t="s">
-        <v>34</v>
-      </c>
-      <c r="G9" t="s">
+      <c r="F9" t="s">
+        <v>93</v>
+      </c>
+      <c r="H9" t="s">
+        <v>64</v>
+      </c>
+      <c r="I9" t="s">
+        <v>65</v>
+      </c>
+      <c r="J9" t="s">
         <v>66</v>
       </c>
-      <c r="H9" t="s">
+      <c r="K9" t="s">
         <v>67</v>
       </c>
-      <c r="I9" t="s">
+      <c r="L9" t="s">
         <v>68</v>
       </c>
-      <c r="J9" t="s">
+      <c r="M9" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
         <v>69</v>
-      </c>
-      <c r="K9" t="s">
-        <v>70</v>
-      </c>
-      <c r="L9" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="10" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>71</v>
       </c>
       <c r="B10" t="s">
         <v>20</v>
       </c>
       <c r="C10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" t="s">
+        <v>31</v>
+      </c>
+      <c r="E10" t="s">
         <v>32</v>
       </c>
-      <c r="D10" t="s">
-        <v>33</v>
-      </c>
-      <c r="E10" t="s">
-        <v>34</v>
-      </c>
-      <c r="G10" t="s">
+      <c r="F10" t="s">
+        <v>96</v>
+      </c>
+      <c r="H10" t="s">
+        <v>70</v>
+      </c>
+      <c r="I10" t="s">
+        <v>71</v>
+      </c>
+      <c r="J10" t="s">
         <v>72</v>
       </c>
-      <c r="H10" t="s">
+      <c r="K10" t="s">
         <v>73</v>
       </c>
-      <c r="I10" t="s">
+    </row>
+    <row r="11" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>74</v>
-      </c>
-      <c r="J10" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="11" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>76</v>
       </c>
       <c r="B11" t="s">
         <v>20</v>
       </c>
       <c r="C11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" t="s">
+        <v>31</v>
+      </c>
+      <c r="E11" t="s">
         <v>32</v>
       </c>
-      <c r="D11" t="s">
-        <v>33</v>
-      </c>
-      <c r="E11" t="s">
-        <v>34</v>
-      </c>
-      <c r="G11" t="s">
+      <c r="F11" t="s">
+        <v>95</v>
+      </c>
+      <c r="H11" t="s">
+        <v>75</v>
+      </c>
+      <c r="I11" t="s">
+        <v>76</v>
+      </c>
+      <c r="J11" t="s">
         <v>77</v>
       </c>
-      <c r="H11" t="s">
+      <c r="K11" t="s">
         <v>78</v>
       </c>
-      <c r="I11" t="s">
+      <c r="L11" t="s">
         <v>79</v>
-      </c>
-      <c r="J11" t="s">
-        <v>80</v>
-      </c>
-      <c r="K11" t="s">
-        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
More Questions and Functionality
</commit_message>
<xml_diff>
--- a/answer_sheets/L4AS.xlsx
+++ b/answer_sheets/L4AS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Caelan\Documents\GitHub\JapaneseSpeechProgram\answer_sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62862919-862D-4DC3-A8FF-2DB3D446288D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63B37BE2-EE39-47FE-A96E-3B56A772D04F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A85B96A8-BC77-4CE1-99B3-3D42F1408ABE}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="177">
   <si>
     <t>はい元気です</t>
   </si>
@@ -95,12 +95,6 @@
     <t>Imananjidesuka (12:30)</t>
   </si>
   <si>
-    <t>Conv</t>
-  </si>
-  <si>
-    <t>Pers</t>
-  </si>
-  <si>
     <t>歳です</t>
   </si>
   <si>
@@ -113,9 +107,6 @@
     <t>LESSON_2</t>
   </si>
   <si>
-    <t>Sorewanandesuka?</t>
-  </si>
-  <si>
     <t>clock_1230.png</t>
   </si>
   <si>
@@ -287,9 +278,6 @@
     <t>GREETINGS</t>
   </si>
   <si>
-    <t xml:space="preserve">Update </t>
-  </si>
-  <si>
     <t>コンピューター</t>
   </si>
   <si>
@@ -333,13 +321,256 @@
   </si>
   <si>
     <t>げんきですか？</t>
+  </si>
+  <si>
+    <t>VOCAB</t>
+  </si>
+  <si>
+    <t>2.wav</t>
+  </si>
+  <si>
+    <t>coffee.png</t>
+  </si>
+  <si>
+    <t>fish.png</t>
+  </si>
+  <si>
+    <t>yen.png</t>
+  </si>
+  <si>
+    <t>LESSON_3</t>
+  </si>
+  <si>
+    <t>coffeeshop.png</t>
+  </si>
+  <si>
+    <t>コーヒー</t>
+  </si>
+  <si>
+    <t>さかな</t>
+  </si>
+  <si>
+    <t>えん</t>
+  </si>
+  <si>
+    <t>.coffee</t>
+  </si>
+  <si>
+    <t>.fish</t>
+  </si>
+  <si>
+    <t>.yen</t>
+  </si>
+  <si>
+    <t>.coffeeshop</t>
+  </si>
+  <si>
+    <t>.computer</t>
+  </si>
+  <si>
+    <t>きっさてん</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>コーヒーです</t>
+  </si>
+  <si>
+    <t>これはコーヒーです</t>
+  </si>
+  <si>
+    <t>魚</t>
+  </si>
+  <si>
+    <t>魚です</t>
+  </si>
+  <si>
+    <t>これは魚です</t>
+  </si>
+  <si>
+    <t>それは魚です</t>
+  </si>
+  <si>
+    <t>それはコーヒーです</t>
+  </si>
+  <si>
+    <t>円です</t>
+  </si>
+  <si>
+    <t>それはお金です</t>
+  </si>
+  <si>
+    <t>これはお金です</t>
+  </si>
+  <si>
+    <t>喫茶店</t>
+  </si>
+  <si>
+    <t>喫茶店です</t>
+  </si>
+  <si>
+    <t>それは 喫茶店です</t>
+  </si>
+  <si>
+    <t>これは 喫茶店です</t>
+  </si>
+  <si>
+    <t>Please respond with これは。。。</t>
+  </si>
+  <si>
+    <t>115, 118</t>
+  </si>
+  <si>
+    <t>49, 50</t>
+  </si>
+  <si>
+    <t>people_descriptions.png</t>
+  </si>
+  <si>
+    <t>takeshisanwachuugokujindesuka?</t>
+  </si>
+  <si>
+    <t>Robaatosanwaamerikajindesuka?</t>
+  </si>
+  <si>
+    <t>Yamashitasenseewakankokujindesuka?</t>
+  </si>
+  <si>
+    <t>Robaatosannosenkoowanihongodesuka?</t>
+  </si>
+  <si>
+    <t>Suusannosenkoowakeezaisesuka?</t>
+  </si>
+  <si>
+    <t>Takeshisanwasakuradaigakunogakuseedesuka?</t>
+  </si>
+  <si>
+    <t>Meariisanwarondondaigakunogakuseedesuka?</t>
+  </si>
+  <si>
+    <t>Takeshisanwaninenseedesuka?</t>
+  </si>
+  <si>
+    <t>Suusanwaichinenseedesuka?</t>
+  </si>
+  <si>
+    <t>Robatosanwayonenseedesuka?</t>
+  </si>
+  <si>
+    <t>placeholder</t>
+  </si>
+  <si>
+    <t>76, 77</t>
+  </si>
+  <si>
+    <t>健さんは日本人です</t>
+  </si>
+  <si>
+    <t>いいえ健さんのは日本人です</t>
+  </si>
+  <si>
+    <t>ロバートはイギリス人です</t>
+  </si>
+  <si>
+    <t>いいえロバートはイギリス人です</t>
+  </si>
+  <si>
+    <t>いいえロバートはイギリス人じゃないです</t>
+  </si>
+  <si>
+    <t>いいえ健さんは中国人じゃないです</t>
+  </si>
+  <si>
+    <t>いいえやました先生は韓国人じゃないです</t>
+  </si>
+  <si>
+    <t>いいえ山下先生は韓国人じゃないです</t>
+  </si>
+  <si>
+    <t>いいえ先生は韓国人じゃないです</t>
+  </si>
+  <si>
+    <t>健さんの選考は歴史です</t>
+  </si>
+  <si>
+    <t>いいえ健さんの線香は日本語じゃないです</t>
+  </si>
+  <si>
+    <t>スーザンの専攻は経済 じゃないです</t>
+  </si>
+  <si>
+    <t>いいえ スザンナ 専攻は経済 じゃないです</t>
+  </si>
+  <si>
+    <t>いいえ スーザンの専攻は経済 じゃないです</t>
+  </si>
+  <si>
+    <t>すーさんの専攻は経済 じゃないです</t>
+  </si>
+  <si>
+    <t>たけしさんは桜大学の学祭です</t>
+  </si>
+  <si>
+    <t>健さんの朝倉大学の学生です</t>
+  </si>
+  <si>
+    <t>武さんは サクラ 大学の学生です</t>
+  </si>
+  <si>
+    <t>はい猛さんの朝倉大学の学生です</t>
+  </si>
+  <si>
+    <t>はい 隆さんの朝倉大学の学生です</t>
+  </si>
+  <si>
+    <t>いいえ メアリーさんはロンドン大学の学生じゃないです</t>
+  </si>
+  <si>
+    <t>いいえ メリーさんのは ロンドン大学の学生じゃないです</t>
+  </si>
+  <si>
+    <t>メリーさんはロンドン大学の学生じゃないです</t>
+  </si>
+  <si>
+    <t>メアリーさんは アリゾナ大学の学生です</t>
+  </si>
+  <si>
+    <t>健成 さんは2年生じゃないです</t>
+  </si>
+  <si>
+    <t>たけしさんのは2年生じゃないです</t>
+  </si>
+  <si>
+    <t>家 健さんのは2年生じゃないです</t>
+  </si>
+  <si>
+    <t>いいえ 健さんのは2年生じゃないです</t>
+  </si>
+  <si>
+    <t>いえいえ 健さんのは2年生じゃないです</t>
+  </si>
+  <si>
+    <t>いいえ スザンヌは1年生じゃないです</t>
+  </si>
+  <si>
+    <t>はい ロバート さんの は 4年生です</t>
+  </si>
+  <si>
+    <t>ロバートさんは4年生です</t>
+  </si>
+  <si>
+    <t>いいえ 山下先生は韓国人じゃないです</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -392,7 +623,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -401,6 +632,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -716,471 +950,933 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4ADC8BB-A32A-472F-9CBF-88915A0B884F}">
-  <dimension ref="A1:V11"/>
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A1:X25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="44.5703125" customWidth="1"/>
-    <col min="2" max="2" width="20.7109375" customWidth="1"/>
-    <col min="3" max="3" width="27" customWidth="1"/>
-    <col min="4" max="21" width="20.7109375" customWidth="1"/>
+    <col min="1" max="1" width="28.5703125" customWidth="1"/>
+    <col min="2" max="2" width="8.85546875" customWidth="1"/>
+    <col min="3" max="3" width="22" customWidth="1"/>
+    <col min="4" max="4" width="14" customWidth="1"/>
+    <col min="5" max="7" width="20.7109375" customWidth="1"/>
+    <col min="8" max="8" width="8.5703125" customWidth="1"/>
+    <col min="9" max="9" width="15.85546875" style="5" customWidth="1"/>
+    <col min="10" max="21" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" ht="15.75">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>20</v>
+        <v>112</v>
       </c>
       <c r="C1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E1" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="F1" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="G1" t="s">
-        <v>99</v>
-      </c>
-      <c r="H1" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="S1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="T1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="S1" t="s">
+      <c r="U1" t="s">
         <v>13</v>
       </c>
-      <c r="T1" t="s">
+      <c r="V1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" ht="15.75">
       <c r="A2" s="1" t="s">
-        <v>26</v>
+        <v>110</v>
       </c>
       <c r="B2" t="s">
-        <v>20</v>
+        <v>112</v>
       </c>
       <c r="C2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D2" t="s">
         <v>23</v>
       </c>
-      <c r="D2" t="s">
-        <v>84</v>
-      </c>
       <c r="E2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F2" t="s">
-        <v>85</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>9</v>
+        <v>81</v>
+      </c>
+      <c r="G2" t="s">
+        <v>128</v>
+      </c>
+      <c r="I2" s="5">
+        <v>60</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>8</v>
       </c>
       <c r="K2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="M2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="N2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="O2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="N2" s="1"/>
-      <c r="O2" s="1"/>
       <c r="P2" s="1"/>
       <c r="Q2" s="1"/>
-    </row>
-    <row r="3" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="R2" s="1"/>
+      <c r="S2" s="1"/>
+    </row>
+    <row r="3" spans="1:24" ht="15.75">
       <c r="A3" s="4" t="s">
         <v>19</v>
       </c>
       <c r="B3" t="s">
-        <v>20</v>
+        <v>112</v>
       </c>
       <c r="C3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" t="s">
         <v>23</v>
       </c>
-      <c r="D3" t="s">
-        <v>25</v>
-      </c>
       <c r="E3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F3" t="s">
-        <v>87</v>
-      </c>
-      <c r="H3" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="J3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="I3" t="s">
+      <c r="K3" t="s">
         <v>17</v>
       </c>
-      <c r="J3" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="L3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24">
       <c r="A4" t="s">
         <v>18</v>
       </c>
       <c r="B4" t="s">
+        <v>113</v>
+      </c>
+      <c r="C4" t="s">
         <v>21</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>23</v>
       </c>
-      <c r="D4" t="s">
-        <v>25</v>
-      </c>
       <c r="E4" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="F4" t="s">
+        <v>84</v>
+      </c>
+      <c r="J4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" ht="15.75">
+      <c r="A5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" t="s">
+        <v>112</v>
+      </c>
+      <c r="C5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F5" t="s">
+        <v>86</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="M5" t="s">
+        <v>33</v>
+      </c>
+      <c r="N5" t="s">
+        <v>34</v>
+      </c>
+      <c r="O5" t="s">
+        <v>35</v>
+      </c>
+      <c r="P5" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>30</v>
+      </c>
+      <c r="R5" t="s">
+        <v>34</v>
+      </c>
+      <c r="S5" t="s">
+        <v>43</v>
+      </c>
+      <c r="T5" t="s">
+        <v>43</v>
+      </c>
+      <c r="U5" t="s">
+        <v>44</v>
+      </c>
+      <c r="V5" t="s">
+        <v>45</v>
+      </c>
+      <c r="W5" t="s">
+        <v>78</v>
+      </c>
+      <c r="X5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" ht="15.75">
+      <c r="A6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" t="s">
+        <v>112</v>
+      </c>
+      <c r="C6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" t="s">
+        <v>29</v>
+      </c>
+      <c r="F6" t="s">
+        <v>87</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="J6" t="s">
+        <v>38</v>
+      </c>
+      <c r="K6" t="s">
+        <v>39</v>
+      </c>
+      <c r="L6" t="s">
+        <v>40</v>
+      </c>
+      <c r="M6" t="s">
+        <v>42</v>
+      </c>
+      <c r="N6" t="s">
+        <v>41</v>
+      </c>
+      <c r="O6" t="s">
+        <v>38</v>
+      </c>
+      <c r="P6" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24" ht="15.75">
+      <c r="A7" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B7" t="s">
+        <v>112</v>
+      </c>
+      <c r="C7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" t="s">
+        <v>29</v>
+      </c>
+      <c r="F7" t="s">
         <v>88</v>
       </c>
-      <c r="H4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5" t="s">
-        <v>30</v>
-      </c>
-      <c r="D5" t="s">
-        <v>31</v>
-      </c>
-      <c r="E5" t="s">
-        <v>32</v>
-      </c>
-      <c r="F5" t="s">
-        <v>90</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="K5" t="s">
-        <v>36</v>
-      </c>
-      <c r="L5" t="s">
-        <v>37</v>
-      </c>
-      <c r="M5" t="s">
-        <v>38</v>
-      </c>
-      <c r="N5" t="s">
-        <v>39</v>
-      </c>
-      <c r="O5" t="s">
-        <v>33</v>
-      </c>
-      <c r="P5" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>46</v>
-      </c>
-      <c r="R5" t="s">
-        <v>46</v>
-      </c>
-      <c r="S5" t="s">
+      <c r="I7" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="J7" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="T5" t="s">
+      <c r="K7" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="U5" t="s">
-        <v>81</v>
-      </c>
-      <c r="V5" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="6" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C6" t="s">
-        <v>30</v>
-      </c>
-      <c r="D6" t="s">
-        <v>31</v>
-      </c>
-      <c r="E6" t="s">
-        <v>32</v>
-      </c>
-      <c r="F6" t="s">
-        <v>91</v>
-      </c>
-      <c r="H6" t="s">
-        <v>41</v>
-      </c>
-      <c r="I6" t="s">
-        <v>42</v>
-      </c>
-      <c r="J6" t="s">
-        <v>43</v>
-      </c>
-      <c r="K6" t="s">
-        <v>45</v>
-      </c>
-      <c r="L6" t="s">
-        <v>44</v>
-      </c>
-      <c r="M6" t="s">
-        <v>41</v>
-      </c>
-      <c r="N6" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="7" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="L7" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7" t="s">
-        <v>30</v>
-      </c>
-      <c r="D7" t="s">
-        <v>31</v>
-      </c>
-      <c r="E7" t="s">
-        <v>32</v>
-      </c>
-      <c r="F7" t="s">
-        <v>92</v>
-      </c>
-      <c r="H7" s="1" t="s">
+      <c r="M7" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="I7" s="1" t="s">
+      <c r="N7" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="J7" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="K7" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="L7" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="M7" s="1"/>
-      <c r="N7" s="1"/>
       <c r="O7" s="1"/>
       <c r="P7" s="1"/>
-    </row>
-    <row r="8" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Q7" s="1"/>
+      <c r="R7" s="1"/>
+    </row>
+    <row r="8" spans="1:24" ht="15.75">
       <c r="A8" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B8" t="s">
+        <v>112</v>
+      </c>
+      <c r="C8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" t="s">
+        <v>29</v>
+      </c>
+      <c r="F8" t="s">
+        <v>90</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="J8" t="s">
+        <v>53</v>
+      </c>
+      <c r="K8" t="s">
+        <v>54</v>
+      </c>
+      <c r="L8" t="s">
         <v>55</v>
       </c>
-      <c r="B8" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" t="s">
-        <v>30</v>
-      </c>
-      <c r="D8" t="s">
-        <v>31</v>
-      </c>
-      <c r="E8" t="s">
-        <v>32</v>
-      </c>
-      <c r="F8" t="s">
-        <v>94</v>
-      </c>
-      <c r="H8" t="s">
+      <c r="M8" t="s">
         <v>56</v>
       </c>
-      <c r="I8" t="s">
+      <c r="N8" t="s">
         <v>57</v>
       </c>
-      <c r="J8" t="s">
+      <c r="O8" t="s">
         <v>58</v>
       </c>
-      <c r="K8" t="s">
+      <c r="P8" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>54</v>
+      </c>
+      <c r="R8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24" ht="15.75">
+      <c r="A9" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="L8" t="s">
+      <c r="B9" t="s">
+        <v>112</v>
+      </c>
+      <c r="C9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" t="s">
+        <v>28</v>
+      </c>
+      <c r="E9" t="s">
+        <v>29</v>
+      </c>
+      <c r="F9" t="s">
+        <v>89</v>
+      </c>
+      <c r="I9" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="J9" t="s">
+        <v>61</v>
+      </c>
+      <c r="K9" t="s">
+        <v>62</v>
+      </c>
+      <c r="L9" t="s">
+        <v>63</v>
+      </c>
+      <c r="M9" t="s">
+        <v>64</v>
+      </c>
+      <c r="N9" t="s">
+        <v>65</v>
+      </c>
+      <c r="O9" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24" ht="15.75">
+      <c r="A10" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B10" t="s">
+        <v>112</v>
+      </c>
+      <c r="C10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" t="s">
+        <v>28</v>
+      </c>
+      <c r="E10" t="s">
+        <v>29</v>
+      </c>
+      <c r="F10" t="s">
+        <v>92</v>
+      </c>
+      <c r="I10" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="J10" t="s">
+        <v>67</v>
+      </c>
+      <c r="K10" t="s">
+        <v>68</v>
+      </c>
+      <c r="L10" t="s">
+        <v>69</v>
+      </c>
+      <c r="M10" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24" ht="15.75">
+      <c r="A11" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B11" t="s">
+        <v>112</v>
+      </c>
+      <c r="C11" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11" t="s">
+        <v>28</v>
+      </c>
+      <c r="E11" t="s">
+        <v>29</v>
+      </c>
+      <c r="F11" t="s">
+        <v>91</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="J11" t="s">
+        <v>72</v>
+      </c>
+      <c r="K11" t="s">
+        <v>73</v>
+      </c>
+      <c r="L11" t="s">
+        <v>74</v>
+      </c>
+      <c r="M11" t="s">
+        <v>75</v>
+      </c>
+      <c r="N11" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="12" spans="1:24" ht="15.75">
+      <c r="A12" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B12" t="s">
+        <v>112</v>
+      </c>
+      <c r="C12" t="s">
+        <v>96</v>
+      </c>
+      <c r="D12" t="s">
+        <v>101</v>
+      </c>
+      <c r="E12" t="s">
+        <v>98</v>
+      </c>
+      <c r="F12" t="s">
+        <v>103</v>
+      </c>
+      <c r="H12" t="s">
+        <v>97</v>
+      </c>
+      <c r="I12" s="5">
+        <v>86</v>
+      </c>
+      <c r="J12" t="s">
+        <v>103</v>
+      </c>
+      <c r="K12" t="s">
+        <v>114</v>
+      </c>
+      <c r="L12" t="s">
+        <v>115</v>
+      </c>
+      <c r="M12" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="13" spans="1:24" ht="15.75">
+      <c r="A13" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B13" t="s">
+        <v>112</v>
+      </c>
+      <c r="D13" t="s">
+        <v>23</v>
+      </c>
+      <c r="E13" t="s">
+        <v>99</v>
+      </c>
+      <c r="F13" t="s">
+        <v>104</v>
+      </c>
+      <c r="H13" t="s">
+        <v>97</v>
+      </c>
+      <c r="I13" s="5">
         <v>60</v>
       </c>
-      <c r="M8" t="s">
-        <v>61</v>
-      </c>
-      <c r="N8" t="s">
-        <v>63</v>
-      </c>
-      <c r="O8" t="s">
-        <v>57</v>
-      </c>
-      <c r="P8" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="9" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="B9" t="s">
-        <v>20</v>
-      </c>
-      <c r="C9" t="s">
-        <v>30</v>
-      </c>
-      <c r="D9" t="s">
-        <v>31</v>
-      </c>
-      <c r="E9" t="s">
-        <v>32</v>
-      </c>
-      <c r="F9" t="s">
-        <v>93</v>
-      </c>
-      <c r="H9" t="s">
-        <v>64</v>
-      </c>
-      <c r="I9" t="s">
-        <v>65</v>
-      </c>
-      <c r="J9" t="s">
-        <v>66</v>
-      </c>
-      <c r="K9" t="s">
-        <v>67</v>
-      </c>
-      <c r="L9" t="s">
-        <v>68</v>
-      </c>
-      <c r="M9" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="10" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="B10" t="s">
-        <v>20</v>
-      </c>
-      <c r="C10" t="s">
-        <v>30</v>
-      </c>
-      <c r="D10" t="s">
-        <v>31</v>
-      </c>
-      <c r="E10" t="s">
-        <v>32</v>
-      </c>
-      <c r="F10" t="s">
-        <v>96</v>
-      </c>
-      <c r="H10" t="s">
-        <v>70</v>
-      </c>
-      <c r="I10" t="s">
-        <v>71</v>
-      </c>
-      <c r="J10" t="s">
-        <v>72</v>
-      </c>
-      <c r="K10" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="11" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="B11" t="s">
-        <v>20</v>
-      </c>
-      <c r="C11" t="s">
-        <v>30</v>
-      </c>
-      <c r="D11" t="s">
-        <v>31</v>
-      </c>
-      <c r="E11" t="s">
-        <v>32</v>
-      </c>
-      <c r="F11" t="s">
-        <v>95</v>
-      </c>
-      <c r="H11" t="s">
-        <v>75</v>
-      </c>
-      <c r="I11" t="s">
-        <v>76</v>
-      </c>
-      <c r="J11" t="s">
-        <v>77</v>
-      </c>
-      <c r="K11" t="s">
-        <v>78</v>
-      </c>
-      <c r="L11" t="s">
-        <v>79</v>
+      <c r="J13" t="s">
+        <v>116</v>
+      </c>
+      <c r="K13" t="s">
+        <v>117</v>
+      </c>
+      <c r="L13" t="s">
+        <v>118</v>
+      </c>
+      <c r="M13" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="14" spans="1:24" ht="15.75">
+      <c r="A14" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B14" t="s">
+        <v>112</v>
+      </c>
+      <c r="D14" t="s">
+        <v>23</v>
+      </c>
+      <c r="E14" t="s">
+        <v>100</v>
+      </c>
+      <c r="F14" t="s">
+        <v>105</v>
+      </c>
+      <c r="H14" t="s">
+        <v>97</v>
+      </c>
+      <c r="I14" s="5">
+        <v>60</v>
+      </c>
+      <c r="J14" t="s">
+        <v>121</v>
+      </c>
+      <c r="K14" t="s">
+        <v>122</v>
+      </c>
+      <c r="L14" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="15" spans="1:24" ht="15.75">
+      <c r="A15" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B15" t="s">
+        <v>112</v>
+      </c>
+      <c r="D15" t="s">
+        <v>23</v>
+      </c>
+      <c r="E15" t="s">
+        <v>102</v>
+      </c>
+      <c r="F15" t="s">
+        <v>111</v>
+      </c>
+      <c r="H15" t="s">
+        <v>97</v>
+      </c>
+      <c r="I15" s="5">
+        <v>60</v>
+      </c>
+      <c r="J15" t="s">
+        <v>124</v>
+      </c>
+      <c r="K15" t="s">
+        <v>125</v>
+      </c>
+      <c r="L15" t="s">
+        <v>126</v>
+      </c>
+      <c r="M15" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="16" spans="1:24" ht="15.75">
+      <c r="A16" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D16" t="s">
+        <v>23</v>
+      </c>
+      <c r="E16" t="s">
+        <v>131</v>
+      </c>
+      <c r="F16" t="s">
+        <v>142</v>
+      </c>
+      <c r="I16" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="J16" t="s">
+        <v>144</v>
+      </c>
+      <c r="K16" t="s">
+        <v>145</v>
+      </c>
+      <c r="L16" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" ht="15.75">
+      <c r="A17" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="D17" t="s">
+        <v>23</v>
+      </c>
+      <c r="E17" t="s">
+        <v>131</v>
+      </c>
+      <c r="F17" t="s">
+        <v>142</v>
+      </c>
+      <c r="I17" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="J17" t="s">
+        <v>146</v>
+      </c>
+      <c r="K17" t="s">
+        <v>147</v>
+      </c>
+      <c r="L17" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" ht="15.75">
+      <c r="A18" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="D18" t="s">
+        <v>23</v>
+      </c>
+      <c r="E18" t="s">
+        <v>131</v>
+      </c>
+      <c r="F18" t="s">
+        <v>142</v>
+      </c>
+      <c r="I18" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="J18" t="s">
+        <v>150</v>
+      </c>
+      <c r="K18" t="s">
+        <v>176</v>
+      </c>
+      <c r="L18" t="s">
+        <v>151</v>
+      </c>
+      <c r="M18" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" ht="15.75">
+      <c r="A19" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="D19" t="s">
+        <v>23</v>
+      </c>
+      <c r="E19" t="s">
+        <v>131</v>
+      </c>
+      <c r="F19" t="s">
+        <v>142</v>
+      </c>
+      <c r="I19" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="J19" t="s">
+        <v>153</v>
+      </c>
+      <c r="K19" t="s">
+        <v>154</v>
+      </c>
+      <c r="M19" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" ht="15.75">
+      <c r="A20" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D20" t="s">
+        <v>23</v>
+      </c>
+      <c r="E20" t="s">
+        <v>131</v>
+      </c>
+      <c r="F20" t="s">
+        <v>142</v>
+      </c>
+      <c r="I20" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="J20" t="s">
+        <v>155</v>
+      </c>
+      <c r="K20" t="s">
+        <v>156</v>
+      </c>
+      <c r="L20" t="s">
+        <v>157</v>
+      </c>
+      <c r="N20" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" ht="15.75">
+      <c r="A21" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D21" t="s">
+        <v>23</v>
+      </c>
+      <c r="E21" t="s">
+        <v>131</v>
+      </c>
+      <c r="F21" t="s">
+        <v>142</v>
+      </c>
+      <c r="I21" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="J21" t="s">
+        <v>159</v>
+      </c>
+      <c r="K21" t="s">
+        <v>160</v>
+      </c>
+      <c r="L21" t="s">
+        <v>161</v>
+      </c>
+      <c r="M21" t="s">
+        <v>160</v>
+      </c>
+      <c r="N21" t="s">
+        <v>162</v>
+      </c>
+      <c r="O21" t="s">
+        <v>163</v>
+      </c>
+      <c r="P21" t="s">
+        <v>162</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" ht="15.75">
+      <c r="A22" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D22" t="s">
+        <v>23</v>
+      </c>
+      <c r="E22" t="s">
+        <v>131</v>
+      </c>
+      <c r="F22" t="s">
+        <v>142</v>
+      </c>
+      <c r="I22" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="J22" t="s">
+        <v>164</v>
+      </c>
+      <c r="K22" t="s">
+        <v>165</v>
+      </c>
+      <c r="L22" t="s">
+        <v>166</v>
+      </c>
+      <c r="N22" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" ht="15.75">
+      <c r="A23" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="D23" t="s">
+        <v>23</v>
+      </c>
+      <c r="E23" t="s">
+        <v>131</v>
+      </c>
+      <c r="F23" t="s">
+        <v>142</v>
+      </c>
+      <c r="I23" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="J23" t="s">
+        <v>168</v>
+      </c>
+      <c r="K23" t="s">
+        <v>169</v>
+      </c>
+      <c r="L23" t="s">
+        <v>170</v>
+      </c>
+      <c r="M23" t="s">
+        <v>171</v>
+      </c>
+      <c r="N23" t="s">
+        <v>171</v>
+      </c>
+      <c r="O23" t="s">
+        <v>169</v>
+      </c>
+      <c r="P23" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" ht="15.75">
+      <c r="A24" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="D24" t="s">
+        <v>23</v>
+      </c>
+      <c r="E24" t="s">
+        <v>131</v>
+      </c>
+      <c r="F24" t="s">
+        <v>142</v>
+      </c>
+      <c r="I24" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="J24" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" ht="15.75">
+      <c r="A25" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="D25" t="s">
+        <v>23</v>
+      </c>
+      <c r="E25" t="s">
+        <v>131</v>
+      </c>
+      <c r="F25" t="s">
+        <v>142</v>
+      </c>
+      <c r="I25" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="J25" t="s">
+        <v>174</v>
+      </c>
+      <c r="K25" t="s">
+        <v>175</v>
       </c>
     </row>
   </sheetData>

</xml_diff>